<commit_message>
Updated resultsGenerator.py,  deprecated resultsTrackerToXlsx.py
Combined resultsGenerator.py and resultsTrackerToXlsx.py to one file, tested and works successfully.  Will update README.md to reflect changes.
</commit_message>
<xml_diff>
--- a/output/summaryOutput.xlsx
+++ b/output/summaryOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="173">
   <si>
     <t>tpGain</t>
   </si>
@@ -82,6 +82,9 @@
     <t>sheet16</t>
   </si>
   <si>
+    <t>sheet17</t>
+  </si>
+  <si>
     <t>sheet18</t>
   </si>
   <si>
@@ -106,18 +109,318 @@
     <t>sheet25</t>
   </si>
   <si>
+    <t>sheet26</t>
+  </si>
+  <si>
     <t>sheet27</t>
   </si>
   <si>
+    <t>sheet28</t>
+  </si>
+  <si>
     <t>sheet29</t>
   </si>
   <si>
+    <t>sheet31</t>
+  </si>
+  <si>
+    <t>sheet32</t>
+  </si>
+  <si>
+    <t>sheet34</t>
+  </si>
+  <si>
+    <t>sheet36</t>
+  </si>
+  <si>
+    <t>sheet37</t>
+  </si>
+  <si>
+    <t>sheet38</t>
+  </si>
+  <si>
+    <t>sheet39</t>
+  </si>
+  <si>
+    <t>sheet40</t>
+  </si>
+  <si>
+    <t>sheet42</t>
+  </si>
+  <si>
+    <t>sheet44</t>
+  </si>
+  <si>
+    <t>sheet45</t>
+  </si>
+  <si>
+    <t>sheet46</t>
+  </si>
+  <si>
+    <t>sheet47</t>
+  </si>
+  <si>
+    <t>sheet48</t>
+  </si>
+  <si>
+    <t>sheet49</t>
+  </si>
+  <si>
+    <t>sheet50</t>
+  </si>
+  <si>
+    <t>sheet51</t>
+  </si>
+  <si>
+    <t>sheet52</t>
+  </si>
+  <si>
+    <t>sheet53</t>
+  </si>
+  <si>
+    <t>sheet54</t>
+  </si>
+  <si>
+    <t>sheet55</t>
+  </si>
+  <si>
+    <t>sheet56</t>
+  </si>
+  <si>
+    <t>sheet57</t>
+  </si>
+  <si>
+    <t>sheet58</t>
+  </si>
+  <si>
+    <t>sheet59</t>
+  </si>
+  <si>
+    <t>sheet60</t>
+  </si>
+  <si>
+    <t>sheet61</t>
+  </si>
+  <si>
+    <t>sheet62</t>
+  </si>
+  <si>
+    <t>sheet63</t>
+  </si>
+  <si>
+    <t>sheet64</t>
+  </si>
+  <si>
+    <t>sheet65</t>
+  </si>
+  <si>
+    <t>sheet66</t>
+  </si>
+  <si>
+    <t>sheet67</t>
+  </si>
+  <si>
+    <t>sheet68</t>
+  </si>
+  <si>
+    <t>sheet69</t>
+  </si>
+  <si>
+    <t>sheet70</t>
+  </si>
+  <si>
+    <t>sheet71</t>
+  </si>
+  <si>
+    <t>sheet72</t>
+  </si>
+  <si>
+    <t>sheet73</t>
+  </si>
+  <si>
+    <t>sheet74</t>
+  </si>
+  <si>
+    <t>sheet75</t>
+  </si>
+  <si>
+    <t>sheet76</t>
+  </si>
+  <si>
+    <t>sheet77</t>
+  </si>
+  <si>
+    <t>sheet78</t>
+  </si>
+  <si>
+    <t>sheet79</t>
+  </si>
+  <si>
+    <t>sheet80</t>
+  </si>
+  <si>
+    <t>sheet81</t>
+  </si>
+  <si>
+    <t>sheet82</t>
+  </si>
+  <si>
+    <t>sheet83</t>
+  </si>
+  <si>
+    <t>sheet84</t>
+  </si>
+  <si>
+    <t>sheet85</t>
+  </si>
+  <si>
+    <t>sheet86</t>
+  </si>
+  <si>
+    <t>sheet88</t>
+  </si>
+  <si>
+    <t>sheet89</t>
+  </si>
+  <si>
+    <t>sheet90</t>
+  </si>
+  <si>
+    <t>sheet91</t>
+  </si>
+  <si>
+    <t>sheet92</t>
+  </si>
+  <si>
+    <t>sheet93</t>
+  </si>
+  <si>
+    <t>sheet94</t>
+  </si>
+  <si>
+    <t>sheet95</t>
+  </si>
+  <si>
+    <t>sheet97</t>
+  </si>
+  <si>
+    <t>sheet99</t>
+  </si>
+  <si>
     <t>long</t>
   </si>
   <si>
     <t>short</t>
   </si>
   <si>
+    <t>2018.08.09</t>
+  </si>
+  <si>
+    <t>2018.02.06</t>
+  </si>
+  <si>
+    <t>2018.02.21</t>
+  </si>
+  <si>
+    <t>2018.03.23</t>
+  </si>
+  <si>
+    <t>2018.05.14</t>
+  </si>
+  <si>
+    <t>2018.03.19</t>
+  </si>
+  <si>
+    <t>2018.05.10</t>
+  </si>
+  <si>
+    <t>2018.03.27</t>
+  </si>
+  <si>
+    <t>2018.04.24</t>
+  </si>
+  <si>
+    <t>2018.12.10</t>
+  </si>
+  <si>
+    <t>2018.04.18</t>
+  </si>
+  <si>
+    <t>2018.11.20</t>
+  </si>
+  <si>
+    <t>2018.06.08</t>
+  </si>
+  <si>
+    <t>2018.06.14</t>
+  </si>
+  <si>
+    <t>2018.07.13</t>
+  </si>
+  <si>
+    <t>2018.06.29</t>
+  </si>
+  <si>
+    <t>2018.06.28</t>
+  </si>
+  <si>
+    <t>2018.11.06</t>
+  </si>
+  <si>
+    <t>2018.10.19</t>
+  </si>
+  <si>
+    <t>2018.08.03</t>
+  </si>
+  <si>
+    <t>2018.08.23</t>
+  </si>
+  <si>
+    <t>2018.10.16</t>
+  </si>
+  <si>
+    <t>2018.10.08</t>
+  </si>
+  <si>
+    <t>2018.12.04</t>
+  </si>
+  <si>
+    <t>2019.04.18</t>
+  </si>
+  <si>
+    <t>2018.12.05</t>
+  </si>
+  <si>
+    <t>2019.01.08</t>
+  </si>
+  <si>
+    <t>2019.02.13</t>
+  </si>
+  <si>
+    <t>2019.01.04</t>
+  </si>
+  <si>
+    <t>2019.04.17</t>
+  </si>
+  <si>
+    <t>2019.09.13</t>
+  </si>
+  <si>
+    <t>2019.04.08</t>
+  </si>
+  <si>
+    <t>2019.04.10</t>
+  </si>
+  <si>
+    <t>2019.03.08</t>
+  </si>
+  <si>
+    <t>2019.03.12</t>
+  </si>
+  <si>
+    <t>2019.04.03</t>
+  </si>
+  <si>
     <t>2019.03.27</t>
   </si>
   <si>
@@ -169,9 +472,6 @@
     <t>2019.08.28</t>
   </si>
   <si>
-    <t>2019.09.13</t>
-  </si>
-  <si>
     <t>2019.10.08</t>
   </si>
   <si>
@@ -182,6 +482,42 @@
   </si>
   <si>
     <t>2019.11.07</t>
+  </si>
+  <si>
+    <t>2018.01.31</t>
+  </si>
+  <si>
+    <t>2018.08.07</t>
+  </si>
+  <si>
+    <t>2018.03.26</t>
+  </si>
+  <si>
+    <t>2018.11.14</t>
+  </si>
+  <si>
+    <t>2018.07.26</t>
+  </si>
+  <si>
+    <t>2018.08.06</t>
+  </si>
+  <si>
+    <t>2018.08.31</t>
+  </si>
+  <si>
+    <t>2019.09.12</t>
+  </si>
+  <si>
+    <t>2019.01.03</t>
+  </si>
+  <si>
+    <t>2019.01.07</t>
+  </si>
+  <si>
+    <t>2019.02.14</t>
+  </si>
+  <si>
+    <t>2019.01.24</t>
   </si>
   <si>
     <t>2019.05.15</t>
@@ -554,7 +890,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -585,13 +921,22 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>0.004089999999999927</v>
+        <v>0.002469999999999972</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>99</v>
+      </c>
+      <c r="E2">
+        <v>-0.0005100000000000104</v>
+      </c>
+      <c r="F2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -599,22 +944,22 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.000280000000000058</v>
+        <v>0.002579999999999805</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="E3">
-        <v>-0.001639999999999864</v>
+        <v>-0.003919999999999924</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -622,22 +967,22 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.003850000000000131</v>
+        <v>0.001159999999999828</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="E4">
-        <v>-0.0021199999999999</v>
+        <v>-0.0002899999999999014</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -645,22 +990,22 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.0003500000000000725</v>
+        <v>0.0009999999999998899</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="E5">
-        <v>-0.001170000000000115</v>
+        <v>-0.004059999999999953</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -668,22 +1013,22 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.0002100000000000435</v>
+        <v>0.005499999999999838</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
       <c r="E6">
-        <v>-0.0002099999999998214</v>
+        <v>-0.0008899999999998354</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -691,22 +1036,22 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.001129999999999853</v>
+        <v>0.00254999999999983</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="E7">
-        <v>-0.002590000000000092</v>
+        <v>-0.003689999999999971</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -714,22 +1059,22 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.001800000000000024</v>
+        <v>0.005269999999999886</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="E8">
-        <v>-0.002499999999999947</v>
+        <v>-0.001309999999999922</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -737,22 +1082,22 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>0.00112000000000001</v>
+        <v>0.0009099999999999664</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="E9">
-        <v>-0.002769999999999939</v>
+        <v>-0.001360000000000028</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -760,22 +1105,22 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>0.001440000000000108</v>
+        <v>0.00378999999999996</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="E10">
-        <v>-0.003989999999999938</v>
+        <v>-0.000180000000000069</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -783,22 +1128,22 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>0.001069999999999904</v>
+        <v>0.002289999999999903</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="E11">
-        <v>-0.001900000000000013</v>
+        <v>-0.005950000000000122</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -806,22 +1151,22 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>0.0003500000000000725</v>
+        <v>0.001720000000000166</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="E12">
-        <v>-0.00266999999999995</v>
+        <v>-0.001870000000000038</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -829,22 +1174,22 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>0.002560000000000118</v>
+        <v>0.002739999999999965</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="E13">
-        <v>-0.0021199999999999</v>
+        <v>-0.001400000000000068</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -852,22 +1197,22 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>0.000420000000000087</v>
+        <v>0.000400000000000178</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="E14">
-        <v>-0.001649999999999929</v>
+        <v>-0.0006600000000001049</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -875,22 +1220,22 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>0.0005299999999999194</v>
+        <v>0.0001700000000000035</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="E15">
-        <v>-0.000340000000000007</v>
+        <v>-0.007479999999999931</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -898,13 +1243,22 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.00275000000000003</v>
+        <v>0.0002099999999998214</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>103</v>
+      </c>
+      <c r="E16">
+        <v>-0.002730000000000121</v>
+      </c>
+      <c r="F16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -912,22 +1266,22 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.0009900000000000464</v>
+        <v>0.0001700000000000035</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="E17">
-        <v>-0.002179999999999849</v>
+        <v>-0.000220000000000109</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="G17" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -935,22 +1289,22 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>0.0005399999999999849</v>
+        <v>0.006839999999999957</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="E18">
-        <v>-0.001340000000000119</v>
+        <v>-0.00340000000000007</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="G18" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -958,13 +1312,22 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>0.00254999999999983</v>
+        <v>0.0004699999999999704</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>113</v>
+      </c>
+      <c r="E19">
+        <v>-0.0005500000000000504</v>
+      </c>
+      <c r="F19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -972,13 +1335,22 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.0005599999999998939</v>
+        <v>0.002550000000000052</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>114</v>
+      </c>
+      <c r="E20">
+        <v>-0.003980000000000095</v>
+      </c>
+      <c r="F20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -986,13 +1358,22 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>0.0009600000000000719</v>
+        <v>0.005700000000000038</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>112</v>
+      </c>
+      <c r="E21">
+        <v>-0.0009099999999999664</v>
+      </c>
+      <c r="F21" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1000,13 +1381,22 @@
         <v>26</v>
       </c>
       <c r="B22">
-        <v>0.005509999999999904</v>
+        <v>0.005900000000000016</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>115</v>
+      </c>
+      <c r="E22">
+        <v>-0.002410000000000023</v>
+      </c>
+      <c r="F22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1014,13 +1404,22 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>0.005449999999999955</v>
+        <v>0.004460000000000131</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>116</v>
+      </c>
+      <c r="E23">
+        <v>-0.001390000000000002</v>
+      </c>
+      <c r="F23" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1028,22 +1427,22 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>0.001330000000000053</v>
+        <v>0.01217999999999986</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="E24">
-        <v>-0.000260000000000149</v>
+        <v>-0.0006099999999999994</v>
       </c>
       <c r="F24" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="G24" t="s">
-        <v>60</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1051,22 +1450,22 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>0.000700000000000145</v>
+        <v>0.002860000000000085</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="E25">
-        <v>-0.0004100000000000215</v>
+        <v>-9.999999999843467e-06</v>
       </c>
       <c r="F25" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="G25" t="s">
-        <v>55</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1074,22 +1473,22 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>0.000480000000000036</v>
+        <v>0.0006200000000000649</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="E26">
-        <v>-0.001020000000000021</v>
+        <v>-0.002140000000000031</v>
       </c>
       <c r="F26" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="G26" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1097,13 +1496,1364 @@
         <v>31</v>
       </c>
       <c r="B27">
+        <v>0.002129999999999965</v>
+      </c>
+      <c r="C27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27">
+        <v>-0.00124000000000013</v>
+      </c>
+      <c r="F27" t="s">
+        <v>97</v>
+      </c>
+      <c r="G27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>0.00448000000000004</v>
+      </c>
+      <c r="C28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28">
+        <v>-0.003570000000000073</v>
+      </c>
+      <c r="F28" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29">
+        <v>0.003040000000000154</v>
+      </c>
+      <c r="C29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29">
+        <v>-0.004070000000000018</v>
+      </c>
+      <c r="F29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30">
+        <v>0.01289000000000007</v>
+      </c>
+      <c r="C30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30">
+        <v>-0.002510000000000012</v>
+      </c>
+      <c r="F30" t="s">
+        <v>97</v>
+      </c>
+      <c r="G30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31">
+        <v>0.003759999999999986</v>
+      </c>
+      <c r="C31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32">
+        <v>0.003509999999999902</v>
+      </c>
+      <c r="C32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33">
+        <v>7.00000000000145e-05</v>
+      </c>
+      <c r="C33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34">
+        <v>0.0005100000000000104</v>
+      </c>
+      <c r="C34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35">
+        <v>0.00116000000000005</v>
+      </c>
+      <c r="C35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36">
+        <v>0.0004999999999999449</v>
+      </c>
+      <c r="C36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37">
+        <v>0.0006800000000000139</v>
+      </c>
+      <c r="C37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38">
+        <v>0.00107999999999997</v>
+      </c>
+      <c r="C38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" t="s">
+        <v>121</v>
+      </c>
+      <c r="E38">
+        <v>-0.002510000000000012</v>
+      </c>
+      <c r="F38" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39">
+        <v>0.00391000000000008</v>
+      </c>
+      <c r="C39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40">
+        <v>0.001829999999999998</v>
+      </c>
+      <c r="C40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41">
+        <v>0.001919999999999922</v>
+      </c>
+      <c r="C41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" t="s">
+        <v>122</v>
+      </c>
+      <c r="E41">
+        <v>-0.003819999999999935</v>
+      </c>
+      <c r="F41" t="s">
+        <v>98</v>
+      </c>
+      <c r="G41" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42">
+        <v>0.000380000000000047</v>
+      </c>
+      <c r="C42" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42">
+        <v>-0.00175000000000014</v>
+      </c>
+      <c r="F42" t="s">
+        <v>97</v>
+      </c>
+      <c r="G42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43">
+        <v>0.001319999999999988</v>
+      </c>
+      <c r="C43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D43" t="s">
+        <v>123</v>
+      </c>
+      <c r="E43">
+        <v>-0.001130000000000075</v>
+      </c>
+      <c r="F43" t="s">
+        <v>97</v>
+      </c>
+      <c r="G43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44">
+        <v>0.002780000000000005</v>
+      </c>
+      <c r="C44" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44">
+        <v>-0.0005500000000000504</v>
+      </c>
+      <c r="F44" t="s">
+        <v>98</v>
+      </c>
+      <c r="G44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45">
+        <v>0.0007099999999999884</v>
+      </c>
+      <c r="C45" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45">
+        <v>-0.000340000000000007</v>
+      </c>
+      <c r="F45" t="s">
+        <v>97</v>
+      </c>
+      <c r="G45" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46">
+        <v>0.0004299999999999304</v>
+      </c>
+      <c r="C46" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46">
+        <v>-0.003230000000000066</v>
+      </c>
+      <c r="F46" t="s">
+        <v>98</v>
+      </c>
+      <c r="G46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47">
+        <v>0.0007399999999999629</v>
+      </c>
+      <c r="C47" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" t="s">
+        <v>126</v>
+      </c>
+      <c r="E47">
+        <v>-0.0001700000000000035</v>
+      </c>
+      <c r="F47" t="s">
+        <v>98</v>
+      </c>
+      <c r="G47" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48">
+        <v>0.0007100000000002105</v>
+      </c>
+      <c r="C48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" t="s">
+        <v>127</v>
+      </c>
+      <c r="E48">
+        <v>-0.002160000000000162</v>
+      </c>
+      <c r="F48" t="s">
+        <v>97</v>
+      </c>
+      <c r="G48" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49">
+        <v>0.001130000000000075</v>
+      </c>
+      <c r="C49" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" t="s">
+        <v>127</v>
+      </c>
+      <c r="E49">
+        <v>-0.002150000000000096</v>
+      </c>
+      <c r="F49" t="s">
+        <v>97</v>
+      </c>
+      <c r="G49" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50">
+        <v>0.001659999999999995</v>
+      </c>
+      <c r="C50" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50">
+        <v>-0.003780000000000117</v>
+      </c>
+      <c r="F50" t="s">
+        <v>97</v>
+      </c>
+      <c r="G50" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51">
+        <v>0.00258999999999987</v>
+      </c>
+      <c r="C51" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" t="s">
+        <v>123</v>
+      </c>
+      <c r="E51">
+        <v>-0.002070000000000016</v>
+      </c>
+      <c r="F51" t="s">
+        <v>97</v>
+      </c>
+      <c r="G51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52">
+        <v>0.003090000000000037</v>
+      </c>
+      <c r="C52" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" t="s">
+        <v>126</v>
+      </c>
+      <c r="E52">
+        <v>-0.001979999999999871</v>
+      </c>
+      <c r="F52" t="s">
+        <v>98</v>
+      </c>
+      <c r="G52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53">
+        <v>0.006299999999999972</v>
+      </c>
+      <c r="C53" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" t="s">
+        <v>129</v>
+      </c>
+      <c r="E53">
+        <v>-0.001599999999999824</v>
+      </c>
+      <c r="F53" t="s">
+        <v>97</v>
+      </c>
+      <c r="G53" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54">
+        <v>0.00266999999999995</v>
+      </c>
+      <c r="C54" t="s">
+        <v>98</v>
+      </c>
+      <c r="D54" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54">
+        <v>-0.005489999999999995</v>
+      </c>
+      <c r="F54" t="s">
+        <v>98</v>
+      </c>
+      <c r="G54" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55">
+        <v>0.000240000000000018</v>
+      </c>
+      <c r="C55" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55">
+        <v>-0.0002100000000000435</v>
+      </c>
+      <c r="F55" t="s">
+        <v>97</v>
+      </c>
+      <c r="G55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56">
+        <v>0.001829999999999998</v>
+      </c>
+      <c r="C56" t="s">
+        <v>97</v>
+      </c>
+      <c r="D56" t="s">
+        <v>131</v>
+      </c>
+      <c r="E56">
+        <v>-0.0006099999999999994</v>
+      </c>
+      <c r="F56" t="s">
+        <v>97</v>
+      </c>
+      <c r="G56" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57">
+        <v>0.002229999999999954</v>
+      </c>
+      <c r="C57" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57" t="s">
+        <v>126</v>
+      </c>
+      <c r="E57">
+        <v>-0.0002099999999998214</v>
+      </c>
+      <c r="F57" t="s">
+        <v>98</v>
+      </c>
+      <c r="G57" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58">
+        <v>0.0005699999999999594</v>
+      </c>
+      <c r="C58" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" t="s">
+        <v>126</v>
+      </c>
+      <c r="E58">
+        <v>-0.0003699999999999815</v>
+      </c>
+      <c r="F58" t="s">
+        <v>98</v>
+      </c>
+      <c r="G58" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59">
+        <v>0.001609999999999889</v>
+      </c>
+      <c r="C59" t="s">
+        <v>98</v>
+      </c>
+      <c r="D59" t="s">
+        <v>132</v>
+      </c>
+      <c r="E59">
+        <v>-0.001390000000000002</v>
+      </c>
+      <c r="F59" t="s">
+        <v>98</v>
+      </c>
+      <c r="G59" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60">
+        <v>0.0007700000000001594</v>
+      </c>
+      <c r="C60" t="s">
+        <v>98</v>
+      </c>
+      <c r="D60" t="s">
+        <v>133</v>
+      </c>
+      <c r="E60">
+        <v>-0.0009099999999999664</v>
+      </c>
+      <c r="F60" t="s">
+        <v>98</v>
+      </c>
+      <c r="G60" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61">
+        <v>0.0007200000000000539</v>
+      </c>
+      <c r="C61" t="s">
+        <v>97</v>
+      </c>
+      <c r="D61" t="s">
+        <v>134</v>
+      </c>
+      <c r="E61">
+        <v>-0.0005100000000000104</v>
+      </c>
+      <c r="F61" t="s">
+        <v>97</v>
+      </c>
+      <c r="G61" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62">
+        <v>0.0005699999999999594</v>
+      </c>
+      <c r="C62" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62" t="s">
+        <v>134</v>
+      </c>
+      <c r="E62">
+        <v>-0.001350000000000184</v>
+      </c>
+      <c r="F62" t="s">
+        <v>97</v>
+      </c>
+      <c r="G62" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63">
+        <v>0.001149999999999984</v>
+      </c>
+      <c r="C63" t="s">
+        <v>98</v>
+      </c>
+      <c r="D63" t="s">
+        <v>132</v>
+      </c>
+      <c r="E63">
+        <v>-0.001759999999999984</v>
+      </c>
+      <c r="F63" t="s">
+        <v>98</v>
+      </c>
+      <c r="G63" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64">
+        <v>0.0007999999999999119</v>
+      </c>
+      <c r="C64" t="s">
+        <v>98</v>
+      </c>
+      <c r="D64" t="s">
+        <v>132</v>
+      </c>
+      <c r="E64">
+        <v>-0.00240000000000018</v>
+      </c>
+      <c r="F64" t="s">
+        <v>98</v>
+      </c>
+      <c r="G64" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65">
+        <v>0.001650000000000151</v>
+      </c>
+      <c r="C65" t="s">
+        <v>98</v>
+      </c>
+      <c r="D65" t="s">
+        <v>133</v>
+      </c>
+      <c r="E65">
+        <v>-0.001309999999999922</v>
+      </c>
+      <c r="F65" t="s">
+        <v>98</v>
+      </c>
+      <c r="G65" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66">
+        <v>0.001560000000000006</v>
+      </c>
+      <c r="C66" t="s">
+        <v>98</v>
+      </c>
+      <c r="D66" t="s">
+        <v>132</v>
+      </c>
+      <c r="E66">
+        <v>-0.003700000000000037</v>
+      </c>
+      <c r="F66" t="s">
+        <v>98</v>
+      </c>
+      <c r="G66" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B67">
+        <v>0.004089999999999927</v>
+      </c>
+      <c r="C67" t="s">
+        <v>97</v>
+      </c>
+      <c r="D67" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68">
+        <v>0.000280000000000058</v>
+      </c>
+      <c r="C68" t="s">
+        <v>98</v>
+      </c>
+      <c r="D68" t="s">
+        <v>136</v>
+      </c>
+      <c r="E68">
+        <v>-0.001639999999999864</v>
+      </c>
+      <c r="F68" t="s">
+        <v>98</v>
+      </c>
+      <c r="G68" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69">
+        <v>0.003850000000000131</v>
+      </c>
+      <c r="C69" t="s">
+        <v>97</v>
+      </c>
+      <c r="D69" t="s">
+        <v>137</v>
+      </c>
+      <c r="E69">
+        <v>-0.0021199999999999</v>
+      </c>
+      <c r="F69" t="s">
+        <v>97</v>
+      </c>
+      <c r="G69" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70">
+        <v>0.0003500000000000725</v>
+      </c>
+      <c r="C70" t="s">
+        <v>98</v>
+      </c>
+      <c r="D70" t="s">
+        <v>138</v>
+      </c>
+      <c r="E70">
+        <v>-0.001170000000000115</v>
+      </c>
+      <c r="F70" t="s">
+        <v>98</v>
+      </c>
+      <c r="G70" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B71">
+        <v>0.0002100000000000435</v>
+      </c>
+      <c r="C71" t="s">
+        <v>97</v>
+      </c>
+      <c r="D71" t="s">
+        <v>139</v>
+      </c>
+      <c r="E71">
+        <v>-0.0002099999999998214</v>
+      </c>
+      <c r="F71" t="s">
+        <v>97</v>
+      </c>
+      <c r="G71" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72">
+        <v>0.001129999999999853</v>
+      </c>
+      <c r="C72" t="s">
+        <v>98</v>
+      </c>
+      <c r="D72" t="s">
+        <v>140</v>
+      </c>
+      <c r="E72">
+        <v>-0.002590000000000092</v>
+      </c>
+      <c r="F72" t="s">
+        <v>98</v>
+      </c>
+      <c r="G72" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73">
+        <v>0.001800000000000024</v>
+      </c>
+      <c r="C73" t="s">
+        <v>97</v>
+      </c>
+      <c r="D73" t="s">
+        <v>141</v>
+      </c>
+      <c r="E73">
+        <v>-0.002499999999999947</v>
+      </c>
+      <c r="F73" t="s">
+        <v>97</v>
+      </c>
+      <c r="G73" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B74">
+        <v>0.00112000000000001</v>
+      </c>
+      <c r="C74" t="s">
+        <v>97</v>
+      </c>
+      <c r="D74" t="s">
+        <v>142</v>
+      </c>
+      <c r="E74">
+        <v>-0.002769999999999939</v>
+      </c>
+      <c r="F74" t="s">
+        <v>97</v>
+      </c>
+      <c r="G74" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75">
+        <v>0.001440000000000108</v>
+      </c>
+      <c r="C75" t="s">
+        <v>97</v>
+      </c>
+      <c r="D75" t="s">
+        <v>139</v>
+      </c>
+      <c r="E75">
+        <v>-0.003989999999999938</v>
+      </c>
+      <c r="F75" t="s">
+        <v>97</v>
+      </c>
+      <c r="G75" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76">
+        <v>0.001069999999999904</v>
+      </c>
+      <c r="C76" t="s">
+        <v>98</v>
+      </c>
+      <c r="D76" t="s">
+        <v>143</v>
+      </c>
+      <c r="E76">
+        <v>-0.001900000000000013</v>
+      </c>
+      <c r="F76" t="s">
+        <v>98</v>
+      </c>
+      <c r="G76" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77">
+        <v>0.0003500000000000725</v>
+      </c>
+      <c r="C77" t="s">
+        <v>97</v>
+      </c>
+      <c r="D77" t="s">
+        <v>144</v>
+      </c>
+      <c r="E77">
+        <v>-0.00266999999999995</v>
+      </c>
+      <c r="F77" t="s">
+        <v>97</v>
+      </c>
+      <c r="G77" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B78">
+        <v>0.002560000000000118</v>
+      </c>
+      <c r="C78" t="s">
+        <v>98</v>
+      </c>
+      <c r="D78" t="s">
+        <v>145</v>
+      </c>
+      <c r="E78">
+        <v>-0.0021199999999999</v>
+      </c>
+      <c r="F78" t="s">
+        <v>98</v>
+      </c>
+      <c r="G78" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B79">
+        <v>0.000420000000000087</v>
+      </c>
+      <c r="C79" t="s">
+        <v>97</v>
+      </c>
+      <c r="D79" t="s">
+        <v>146</v>
+      </c>
+      <c r="E79">
+        <v>-0.001649999999999929</v>
+      </c>
+      <c r="F79" t="s">
+        <v>97</v>
+      </c>
+      <c r="G79" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80">
+        <v>0.0005299999999999194</v>
+      </c>
+      <c r="C80" t="s">
+        <v>98</v>
+      </c>
+      <c r="D80" t="s">
+        <v>147</v>
+      </c>
+      <c r="E80">
+        <v>-0.000340000000000007</v>
+      </c>
+      <c r="F80" t="s">
+        <v>98</v>
+      </c>
+      <c r="G80" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81">
+        <v>0.00275000000000003</v>
+      </c>
+      <c r="C81" t="s">
+        <v>97</v>
+      </c>
+      <c r="D81" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B82">
+        <v>0.0009900000000000464</v>
+      </c>
+      <c r="C82" t="s">
+        <v>97</v>
+      </c>
+      <c r="D82" t="s">
+        <v>148</v>
+      </c>
+      <c r="E82">
+        <v>-0.002179999999999849</v>
+      </c>
+      <c r="F82" t="s">
+        <v>97</v>
+      </c>
+      <c r="G82" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B83">
+        <v>0.0005399999999999849</v>
+      </c>
+      <c r="C83" t="s">
+        <v>98</v>
+      </c>
+      <c r="D83" t="s">
+        <v>149</v>
+      </c>
+      <c r="E83">
+        <v>-0.001340000000000119</v>
+      </c>
+      <c r="F83" t="s">
+        <v>98</v>
+      </c>
+      <c r="G83" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B84">
+        <v>0.00254999999999983</v>
+      </c>
+      <c r="C84" t="s">
+        <v>97</v>
+      </c>
+      <c r="D84" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85">
+        <v>0.0005599999999998939</v>
+      </c>
+      <c r="C85" t="s">
+        <v>97</v>
+      </c>
+      <c r="D85" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B86">
+        <v>0.0009600000000000719</v>
+      </c>
+      <c r="C86" t="s">
+        <v>97</v>
+      </c>
+      <c r="D86" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87">
+        <v>0.005509999999999904</v>
+      </c>
+      <c r="C87" t="s">
+        <v>97</v>
+      </c>
+      <c r="D87" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B88">
+        <v>0.005449999999999955</v>
+      </c>
+      <c r="C88" t="s">
+        <v>97</v>
+      </c>
+      <c r="D88" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89">
+        <v>0.001330000000000053</v>
+      </c>
+      <c r="C89" t="s">
+        <v>98</v>
+      </c>
+      <c r="D89" t="s">
+        <v>152</v>
+      </c>
+      <c r="E89">
+        <v>-0.000260000000000149</v>
+      </c>
+      <c r="F89" t="s">
+        <v>98</v>
+      </c>
+      <c r="G89" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90">
+        <v>0.000700000000000145</v>
+      </c>
+      <c r="C90" t="s">
+        <v>98</v>
+      </c>
+      <c r="D90" t="s">
+        <v>153</v>
+      </c>
+      <c r="E90">
+        <v>-0.0004100000000000215</v>
+      </c>
+      <c r="F90" t="s">
+        <v>98</v>
+      </c>
+      <c r="G90" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B91">
+        <v>0.000480000000000036</v>
+      </c>
+      <c r="C91" t="s">
+        <v>97</v>
+      </c>
+      <c r="D91" t="s">
+        <v>154</v>
+      </c>
+      <c r="E91">
+        <v>-0.001020000000000021</v>
+      </c>
+      <c r="F91" t="s">
+        <v>97</v>
+      </c>
+      <c r="G91" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92">
         <v>0.001300000000000079</v>
       </c>
-      <c r="C27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" t="s">
-        <v>55</v>
+      <c r="C92" t="s">
+        <v>97</v>
+      </c>
+      <c r="D92" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>